<commit_message>
fix indexddb bug, error handling
</commit_message>
<xml_diff>
--- a/app/workbooks/PY - LOCAL.xlsx
+++ b/app/workbooks/PY - LOCAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Code\python\app\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED7206-EC26-48A9-BC87-AF31A3A15BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270E5FB-B7C2-471F-8908-34CFA5320FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve"> =LOCAL.PY(code, data1, data2)</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>https://localhost:4000/test/simple.ipynb</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>https://gist.githubusercontent.com/bolleman/14e68b8d6a6e2897ef5f70dbd28ea7e3/raw/d2ea53a39d90328d96c79e2e46dbc3521d2a757c/emails.py</t>
+  </si>
+  <si>
+    <t>joe@blah.com  and some other text</t>
+  </si>
+  <si>
+    <t>https://whistlernetworks-my.sharepoint.com/:u:/g/personal/brent_boardflare_com/EWmLkixSm1xNsz1NacNt7E4B5Jlic2jDWoenNSzzmsX5tA?download=1</t>
+  </si>
+  <si>
+    <t>https://gist.githubusercontent.com/bolleman/14e68b8d6a6e2897ef5f70dbd28ea7e3/raw/d2ea53a39d90328d96c79e2e46dbc3521d2a757c/email.py</t>
   </si>
 </sst>
 </file>
@@ -673,18 +694,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79FED09-B0DD-4548-A669-E549CAB72C9F}">
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="41.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" customWidth="1"/>
     <col min="7" max="7" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -761,20 +782,79 @@
         <v>Error, see console for details.</v>
       </c>
     </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" cm="1">
+        <f t="array" ref="E10:F10">_xldudf_LOCAL_PY_BETA("text/fuzzy_distance.ipynb",C10,D10:D11,"jaccard")</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.625</v>
+      </c>
+    </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" t="str" cm="1">
         <f t="array" ref="B11">_xldudf_LOCAL_PY_BETA("email.py")</f>
         <v>support2@example.com</v>
       </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D15" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D16" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D17" t="str" cm="1">
+        <f t="array" ref="D17">_xldudf_LOCAL_PY_BETA(D15,D16)</f>
+        <v>joe@blah.com</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D20" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D21" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D22" t="str" cm="1">
+        <f t="array" ref="D22">_xldudf_LOCAL_PY_BETA(D20,D21)</f>
+        <v>Error, see console for details.</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{AB540E7B-3214-4702-ACE2-615C7B28BB9B}"/>
+    <hyperlink ref="D16" r:id="rId2" xr:uid="{CCC0BE0C-43E7-44F9-8BBE-856376C7548E}"/>
+    <hyperlink ref="D21" r:id="rId3" xr:uid="{9B0E2771-B988-4B6F-8C9C-CE6CEE931DAF}"/>
+    <hyperlink ref="D20" r:id="rId4" xr:uid="{C32F8C2C-839A-41AB-8328-0EF465190873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>